<commit_message>
Replace 24 by 23:59 and add warning
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="accepted papers" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11208" uniqueCount="1521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11209" uniqueCount="1524">
   <si>
     <t xml:space="preserve">Paper ID</t>
   </si>
@@ -4442,6 +4442,9 @@
     <t xml:space="preserve">Utah State University</t>
   </si>
   <si>
+    <t xml:space="preserve">[6:00,23:59]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[0,9]</t>
   </si>
   <si>
@@ -4567,7 +4570,13 @@
     <t xml:space="preserve">SN</t>
   </si>
   <si>
-    <t xml:space="preserve">[22,8]</t>
+    <t xml:space="preserve">[22:00,23:59]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[22:00,23:59],[0,8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,8]</t>
   </si>
   <si>
     <t xml:space="preserve">na1</t>
@@ -5203,11 +5212,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.219387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7838,32 +7847,31 @@
   <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="AH33" activeCellId="0" sqref="AH33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.93877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.6275510204082"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.69897959183673"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8823,7 +8831,7 @@
         <v>360</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>10</v>
@@ -8865,7 +8873,7 @@
         <v>537</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="Q10" s="7" t="s">
         <v>1014</v>
@@ -9795,7 +9803,7 @@
         <v>468</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="C19" s="32" t="n">
         <v>10</v>
@@ -9807,7 +9815,7 @@
         <v>112</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="G19" s="32" t="n">
         <v>8</v>
@@ -9831,7 +9839,7 @@
         <v>917</v>
       </c>
       <c r="N19" s="33" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="O19" s="32" t="n">
         <v>687</v>
@@ -9843,7 +9851,7 @@
         <v>917</v>
       </c>
       <c r="R19" s="33" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="S19" s="34"/>
       <c r="T19" s="33" t="s">
@@ -9888,14 +9896,14 @@
         <v>-7</v>
       </c>
       <c r="AH19" s="31" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="AI19" s="31" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="AJ19" s="18"/>
       <c r="AK19" s="31" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10547,7 +10555,7 @@
         <v>482</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="C26" s="55" t="n">
         <v>10</v>
@@ -10589,20 +10597,20 @@
         <v>706</v>
       </c>
       <c r="P26" s="39" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="Q26" s="39" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="R26" s="56" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="S26" s="39"/>
       <c r="T26" s="39" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="U26" s="39" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="V26" s="39"/>
       <c r="W26" s="39"/>
@@ -11292,7 +11300,7 @@
         <v>459</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="C33" s="49" t="n">
         <v>10</v>
@@ -11334,22 +11342,22 @@
         <v>672</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="Q33" s="50" t="s">
+        <v>1486</v>
+      </c>
+      <c r="R33" s="50" t="s">
+        <v>1487</v>
+      </c>
+      <c r="S33" s="50" t="s">
+        <v>1488</v>
+      </c>
+      <c r="T33" s="50" t="s">
         <v>1485</v>
       </c>
-      <c r="R33" s="50" t="s">
+      <c r="U33" s="50" t="s">
         <v>1486</v>
-      </c>
-      <c r="S33" s="50" t="s">
-        <v>1487</v>
-      </c>
-      <c r="T33" s="50" t="s">
-        <v>1484</v>
-      </c>
-      <c r="U33" s="50" t="s">
-        <v>1485</v>
       </c>
       <c r="V33" s="50"/>
       <c r="W33" s="50"/>
@@ -11387,12 +11395,14 @@
         <v>10</v>
       </c>
       <c r="AH33" s="10" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="AI33" s="10" t="s">
-        <v>1488</v>
-      </c>
-      <c r="AJ33" s="12"/>
+        <v>1490</v>
+      </c>
+      <c r="AJ33" s="12" t="s">
+        <v>1491</v>
+      </c>
       <c r="AK33" s="6" t="s">
         <v>1029</v>
       </c>
@@ -12069,27 +12079,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.05612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.08163265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="36" min="34" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13477,7 +13487,7 @@
         <v>7</v>
       </c>
       <c r="AG13" s="6" t="s">
-        <v>1489</v>
+        <v>1492</v>
       </c>
       <c r="AH13" s="12"/>
       <c r="AI13" s="12"/>
@@ -13583,7 +13593,7 @@
         <v>8</v>
       </c>
       <c r="AG14" s="6" t="s">
-        <v>1490</v>
+        <v>1493</v>
       </c>
       <c r="AH14" s="12"/>
       <c r="AI14" s="12"/>
@@ -13685,7 +13695,7 @@
         <v>9</v>
       </c>
       <c r="AG15" s="6" t="s">
-        <v>1491</v>
+        <v>1494</v>
       </c>
       <c r="AH15" s="12"/>
       <c r="AI15" s="12"/>
@@ -13785,7 +13795,7 @@
         <v>1</v>
       </c>
       <c r="AG16" s="14" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="AH16" s="14" t="s">
         <v>316</v>
@@ -18045,28 +18055,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6020408163265"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.20408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.66326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.57142857142857"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="36" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.63265306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="4.39285714285714"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="36" min="34" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="24.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18864,7 +18874,7 @@
         <v>48</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>1493</v>
+        <v>1496</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>50</v>
@@ -19512,7 +19522,7 @@
         <v>48</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>1493</v>
+        <v>1496</v>
       </c>
       <c r="S14" s="7" t="s">
         <v>50</v>
@@ -19836,7 +19846,7 @@
         <v>159</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>161</v>
@@ -19883,7 +19893,7 @@
         <v>2</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>1495</v>
+        <v>1498</v>
       </c>
       <c r="AI17" s="1" t="s">
         <v>280</v>
@@ -20006,7 +20016,7 @@
         <v>464</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>12</v>
@@ -20045,25 +20055,25 @@
         <v>157</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>1497</v>
+        <v>1500</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>1498</v>
+        <v>1501</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>1500</v>
+        <v>1503</v>
       </c>
       <c r="S19" s="15" t="s">
+        <v>1504</v>
+      </c>
+      <c r="T19" s="15" t="s">
         <v>1501</v>
       </c>
-      <c r="T19" s="15" t="s">
-        <v>1498</v>
-      </c>
       <c r="U19" s="15" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
       <c r="V19" s="16"/>
       <c r="W19" s="16"/>
@@ -20835,10 +20845,10 @@
         <v>9</v>
       </c>
       <c r="AH26" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI26" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ26" s="12"/>
       <c r="AK26" s="6" t="s">
@@ -20943,10 +20953,10 @@
         <v>9</v>
       </c>
       <c r="AH27" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI27" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ27" s="12"/>
       <c r="AK27" s="6" t="s">
@@ -21326,7 +21336,7 @@
         <v>100</v>
       </c>
       <c r="R31" s="15" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="S31" s="15" t="s">
         <v>102</v>
@@ -21864,7 +21874,7 @@
         <v>175</v>
       </c>
       <c r="R36" s="15" t="s">
-        <v>1503</v>
+        <v>1506</v>
       </c>
       <c r="S36" s="16"/>
       <c r="T36" s="15" t="s">
@@ -22409,28 +22419,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.57142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.69897959183673"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.38775510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.51530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.63265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.66326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.39285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="3.17857142857143"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="5.5969387755102"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="18.4285714285714"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.1734693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="35" min="33" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.5051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23438,7 +23447,7 @@
         <v>230</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>232</v>
@@ -23756,7 +23765,7 @@
         <v>135</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>1505</v>
+        <v>1508</v>
       </c>
       <c r="S13" s="12"/>
       <c r="T13" s="6" t="s">
@@ -24724,30 +24733,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.51530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.78061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.69897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.8673469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.08163265306122"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.51530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.14795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2142857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="3.17857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="5.93877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.63265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="21" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="5.5969387755102"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.17857142857143"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.63265306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.98469387755102"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25477,10 +25486,10 @@
         <v>9</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ7" s="12"/>
       <c r="AK7" s="6" t="s">
@@ -25807,7 +25816,7 @@
         <v>465</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>1506</v>
+        <v>1509</v>
       </c>
       <c r="C11" s="49" t="n">
         <v>16</v>
@@ -25849,27 +25858,27 @@
         <v>684</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="Q11" s="50" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="R11" s="50" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
       <c r="S11" s="61"/>
       <c r="T11" s="50" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="U11" s="50" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="V11" s="61"/>
       <c r="W11" s="61"/>
       <c r="X11" s="61"/>
       <c r="Y11" s="61"/>
       <c r="Z11" s="10" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="AA11" s="6" t="n">
         <v>15</v>
@@ -26430,7 +26439,7 @@
         <v>466</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>1511</v>
+        <v>1514</v>
       </c>
       <c r="C17" s="49" t="n">
         <v>16</v>
@@ -26472,22 +26481,22 @@
         <v>685</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="Q17" s="50" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="R17" s="50" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="S17" s="50" t="s">
         <v>296</v>
       </c>
       <c r="T17" s="50" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="U17" s="50" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="V17" s="61"/>
       <c r="W17" s="61"/>
@@ -26535,7 +26544,7 @@
         <v>509</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
       <c r="C18" s="49" t="n">
         <v>16</v>
@@ -26577,20 +26586,20 @@
         <v>686</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="Q18" s="50" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
       <c r="R18" s="50" t="s">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="S18" s="61"/>
       <c r="T18" s="50" t="s">
-        <v>1519</v>
+        <v>1522</v>
       </c>
       <c r="U18" s="50" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
       <c r="V18" s="61"/>
       <c r="W18" s="61"/>
@@ -26599,7 +26608,7 @@
       </c>
       <c r="Y18" s="61"/>
       <c r="Z18" s="10" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="AA18" s="6" t="n">
         <v>15</v>
@@ -27381,7 +27390,7 @@
         <v>469</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="C26" s="32" t="n">
         <v>16</v>
@@ -27429,7 +27438,7 @@
         <v>917</v>
       </c>
       <c r="R26" s="33" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="S26" s="34"/>
       <c r="T26" s="33" t="s">
@@ -27472,10 +27481,10 @@
         <v>-7</v>
       </c>
       <c r="AH26" s="31" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="AI26" s="31" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="AJ26" s="18"/>
       <c r="AK26" s="14" t="s">
@@ -28109,22 +28118,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.08163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="28" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.6428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48713,25 +48722,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.8673469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.69897959183673"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="3.57142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.17857142857143"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="4.39285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49390,27 +49399,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.51530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.81122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="3.03061224489796"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.8673469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.1734693877551"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.22448979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53361,33 +53370,33 @@
   </sheetPr>
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="AH15" activeCellId="0" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.25"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.63265306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="3.57142857142857"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54340,7 +54349,7 @@
         <v>1220</v>
       </c>
       <c r="AJ9" s="14" t="s">
-        <v>1221</v>
+        <v>1448</v>
       </c>
       <c r="AK9" s="14" t="s">
         <v>290</v>
@@ -54478,26 +54487,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.44897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2908163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.14795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.25"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.49489795918367"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.83673469387755"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55230,10 +55239,10 @@
         <v>9</v>
       </c>
       <c r="AH7" s="14" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI7" s="14" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ7" s="18"/>
       <c r="AK7" s="14" t="s">
@@ -55340,10 +55349,10 @@
         <v>9</v>
       </c>
       <c r="AH8" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI8" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ8" s="12"/>
       <c r="AK8" s="6" t="s">
@@ -55448,10 +55457,10 @@
         <v>9</v>
       </c>
       <c r="AH9" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI9" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ9" s="12"/>
       <c r="AK9" s="6" t="s">
@@ -55556,10 +55565,10 @@
         <v>9</v>
       </c>
       <c r="AH10" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI10" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ10" s="12"/>
       <c r="AK10" s="6" t="s">
@@ -55806,30 +55815,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.66326530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="6" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="1.81632653061225"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.78061224489796"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="6" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="2.08673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.2142857142857"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.11734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.78061224489796"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.2602040816327"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.4132653061224"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="12.2142857142857"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57009,7 +57018,7 @@
         <v>1</v>
       </c>
       <c r="AG11" s="14" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="AH11" s="18"/>
       <c r="AI11" s="14" t="s">
@@ -57115,7 +57124,7 @@
         <v>2</v>
       </c>
       <c r="AG12" s="14" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="AH12" s="14" t="s">
         <v>310</v>
@@ -57548,10 +57557,10 @@
         <v>2</v>
       </c>
       <c r="AH16" s="10" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="AJ16" s="12"/>
       <c r="AK16" s="12"/>
@@ -58012,7 +58021,7 @@
   </sheetPr>
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="AH39" activeCellId="0" sqref="AH39"/>
@@ -58020,27 +58029,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="1.96428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.14795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6224489795918"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.8673469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="35" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.83673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.95408163265306"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="33" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="6.27040816326531"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="11.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59676,13 +59684,13 @@
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M16" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N16" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O16" s="7" t="n">
         <v>633</v>
@@ -59772,13 +59780,13 @@
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M17" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N17" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O17" s="7" t="n">
         <v>635</v>
@@ -59868,13 +59876,13 @@
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M18" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O18" s="7" t="n">
         <v>636</v>
@@ -59964,13 +59972,13 @@
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M19" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O19" s="7" t="n">
         <v>638</v>
@@ -60060,13 +60068,13 @@
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M20" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N20" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O20" s="7" t="n">
         <v>640</v>
@@ -60156,13 +60164,13 @@
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M21" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N21" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O21" s="7" t="n">
         <v>642</v>
@@ -60254,13 +60262,13 @@
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="6" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M22" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N22" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>1452</v>
       </c>
       <c r="O22" s="7" t="n">
         <v>645</v>
@@ -60352,13 +60360,13 @@
       </c>
       <c r="K23" s="16"/>
       <c r="L23" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M23" s="15" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N23" s="15" t="s">
         <v>1453</v>
-      </c>
-      <c r="N23" s="15" t="s">
-        <v>1452</v>
       </c>
       <c r="O23" s="15" t="n">
         <v>646</v>
@@ -60450,13 +60458,13 @@
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M24" s="15" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N24" s="15" t="s">
         <v>1453</v>
-      </c>
-      <c r="N24" s="15" t="s">
-        <v>1452</v>
       </c>
       <c r="O24" s="15" t="n">
         <v>650</v>
@@ -60548,13 +60556,13 @@
       </c>
       <c r="K25" s="16"/>
       <c r="L25" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M25" s="15" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N25" s="15" t="s">
         <v>1453</v>
-      </c>
-      <c r="N25" s="15" t="s">
-        <v>1452</v>
       </c>
       <c r="O25" s="15" t="n">
         <v>655</v>
@@ -60646,13 +60654,13 @@
       </c>
       <c r="K26" s="16"/>
       <c r="L26" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M26" s="15" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N26" s="15" t="s">
         <v>1453</v>
-      </c>
-      <c r="N26" s="15" t="s">
-        <v>1452</v>
       </c>
       <c r="O26" s="15" t="n">
         <v>659</v>
@@ -60744,13 +60752,13 @@
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M27" s="15" t="s">
+        <v>1454</v>
+      </c>
+      <c r="N27" s="15" t="s">
         <v>1453</v>
-      </c>
-      <c r="N27" s="15" t="s">
-        <v>1452</v>
       </c>
       <c r="O27" s="15" t="n">
         <v>664</v>
@@ -60816,7 +60824,7 @@
         <v>462</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="C28" s="32" t="n">
         <v>8</v>
@@ -60844,7 +60852,7 @@
       </c>
       <c r="K28" s="34"/>
       <c r="L28" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
@@ -60852,7 +60860,7 @@
         <v>676</v>
       </c>
       <c r="P28" s="31" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="Q28" s="33" t="s">
         <v>510</v>
@@ -60862,10 +60870,10 @@
         <v>502</v>
       </c>
       <c r="T28" s="33" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="U28" s="33" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="V28" s="34"/>
       <c r="W28" s="34"/>
@@ -60910,7 +60918,7 @@
         <v>463</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="C29" s="32" t="n">
         <v>8</v>
@@ -60938,7 +60946,7 @@
       </c>
       <c r="K29" s="34"/>
       <c r="L29" s="14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="M29" s="34"/>
       <c r="N29" s="34"/>
@@ -60946,20 +60954,20 @@
         <v>679</v>
       </c>
       <c r="P29" s="31" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="Q29" s="33" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="R29" s="34"/>
       <c r="S29" s="33" t="s">
         <v>502</v>
       </c>
       <c r="T29" s="33" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="U29" s="33" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="V29" s="34"/>
       <c r="W29" s="34"/>
@@ -61430,7 +61438,7 @@
         <v>522</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="C34" s="32" t="n">
         <v>8</v>
@@ -61472,7 +61480,7 @@
         <v>369</v>
       </c>
       <c r="P34" s="31" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="Q34" s="33" t="s">
         <v>386</v>
@@ -62074,7 +62082,7 @@
         <v>511</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C40" s="49" t="n">
         <v>8</v>
@@ -62116,20 +62124,20 @@
         <v>498</v>
       </c>
       <c r="P40" s="10" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="Q40" s="50" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="R40" s="51" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="S40" s="10"/>
       <c r="T40" s="52" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="U40" s="50" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="V40" s="10"/>
       <c r="W40" s="10"/>
@@ -62222,7 +62230,7 @@
         <v>580</v>
       </c>
       <c r="P41" s="6" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="Q41" s="7" t="s">
         <v>473</v>
@@ -62411,26 +62419,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.66326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.08673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.35714285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.73469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.35714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="25" min="17" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.66326530612245"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="0.403061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.22959183673469"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9897959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.81122448979592"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="2.49489795918367"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63163,10 +63170,10 @@
         <v>8</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="AJ7" s="12"/>
       <c r="AK7" s="6" t="s">
@@ -63502,7 +63509,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="C11" s="15" t="n">
         <v>9</v>
@@ -63544,7 +63551,7 @@
         <v>138</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="Q11" s="15" t="s">
         <v>1077</v>
@@ -63556,10 +63563,10 @@
         <v>450</v>
       </c>
       <c r="T11" s="15" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="U11" s="15" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="V11" s="16"/>
       <c r="W11" s="16"/>

</xml_diff>